<commit_message>
chore(EM): fix ui spacing in English locale
</commit_message>
<xml_diff>
--- a/Emmersive/package/LangMod/EN/emmersive_localizations_en.xlsx
+++ b/Emmersive/package/LangMod/EN/emmersive_localizations_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WorkSpace\GameMods\Elin.Plugins\Emmersive\package\LangMod\EN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2584D34-0FCB-43F0-936B-4D9A610624B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6080E8F5-5DE6-4D5A-A3F6-B12D201D9E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="2115" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10965" yWindow="2460" windowWidth="26220" windowHeight="15975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="1" r:id="rId1"/>
@@ -806,12 +806,6 @@
     <t>System Prompt</t>
   </si>
   <si>
-    <t>Character Background</t>
-  </si>
-  <si>
-    <t>Character Relationships</t>
-  </si>
-  <si>
     <t>Character Relationships on the Current Map</t>
   </si>
   <si>
@@ -900,6 +894,12 @@
   </si>
   <si>
     <t>Recent Requests</t>
+  </si>
+  <si>
+    <t>Relationships</t>
+  </si>
+  <si>
+    <t>Backgrounds</t>
   </si>
 </sst>
 </file>
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:XFC110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A77" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D102" sqref="D102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="23.25"/>
@@ -2269,10 +2269,10 @@
         <v>227</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="92" spans="1:4">
@@ -2313,10 +2313,10 @@
         <v>234</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="96" spans="1:4">
@@ -2338,7 +2338,7 @@
         <v>238</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>254</v>
+        <v>285</v>
       </c>
     </row>
     <row r="98" spans="1:4">
@@ -2360,7 +2360,7 @@
         <v>222</v>
       </c>
       <c r="D99" s="4" t="s">
-        <v>255</v>
+        <v>284</v>
       </c>
     </row>
     <row r="100" spans="1:4">
@@ -2371,7 +2371,7 @@
         <v>243</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -2382,7 +2382,7 @@
         <v>245</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="102" spans="1:4">
@@ -2398,90 +2398,90 @@
     </row>
     <row r="103" spans="1:4">
       <c r="A103" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="104" spans="1:4">
       <c r="A104" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D104" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D105" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D106" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D107" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D108" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C109" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="D109" s="4" t="s">
         <v>280</v>
-      </c>
-      <c r="D109" s="4" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="110" spans="1:4">
       <c r="A110" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="D110" s="4" t="s">
         <v>283</v>
-      </c>
-      <c r="C110" s="4" t="s">
-        <v>284</v>
-      </c>
-      <c r="D110" s="4" t="s">
-        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>